<commit_message>
add LR and SVM
</commit_message>
<xml_diff>
--- a/images/accuracy.xlsx
+++ b/images/accuracy.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9347" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9347" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ink" sheetId="1" r:id="rId1"/>
     <sheet name="con" sheetId="2" r:id="rId2"/>
     <sheet name="combined" sheetId="3" r:id="rId3"/>
+    <sheet name="LR" sheetId="5" r:id="rId4"/>
+    <sheet name="SVM" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="4">
   <si>
     <t>label</t>
   </si>
@@ -35,10 +37,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -50,19 +52,42 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
@@ -77,9 +102,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -93,17 +148,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -111,83 +189,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,13 +204,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -220,25 +354,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -250,7 +372,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -262,127 +384,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,56 +395,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -465,7 +417,55 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,9 +487,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,145 +503,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1233,8 +1235,8 @@
   <sheetPr/>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="A1:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -1344,4 +1346,237 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="7.55555555555556" customWidth="1"/>
+    <col min="2" max="2" width="17.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.958241758241758</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.966311197285506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.873097826086956</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.856509261674928</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.899358795650961</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.806461262339216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.945953360768175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.905855042558679</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.824531992176585</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.875609756097561</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0.892837837837837</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="21.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0.98543956043956</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.983761512360639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>0.947282608695652</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.924341247064962</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>0.958182325062726</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.945857014657493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.976131687242798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.941191643022955</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>0.928192232467169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.926829268292683</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>0.951972972972973</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>